<commit_message>
added: data for AI mid prb2
</commit_message>
<xml_diff>
--- a/MidAI.xlsx
+++ b/MidAI.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Problem1" sheetId="1" r:id="rId1"/>
+    <sheet name="Romania" sheetId="2" r:id="rId2"/>
+    <sheet name="Heuristic" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>A</t>
   </si>
@@ -49,17 +51,95 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>VerticeA</t>
+  </si>
+  <si>
+    <t>VerticeB</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Oradea</t>
+  </si>
+  <si>
+    <t>Zerind</t>
+  </si>
+  <si>
+    <t>Sibiu</t>
+  </si>
+  <si>
+    <t>Arad</t>
+  </si>
+  <si>
+    <t>Timisoara</t>
+  </si>
+  <si>
+    <t>Lugoj</t>
+  </si>
+  <si>
+    <t>Mehadia</t>
+  </si>
+  <si>
+    <t>Dobreta</t>
+  </si>
+  <si>
+    <t>Craiova</t>
+  </si>
+  <si>
+    <t>Fagaras</t>
+  </si>
+  <si>
+    <t>Rimnicu Vilcea</t>
+  </si>
+  <si>
+    <t>Pitesti</t>
+  </si>
+  <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
+    <t>Urziceni</t>
+  </si>
+  <si>
+    <t>Hirsova</t>
+  </si>
+  <si>
+    <t>Eforie</t>
+  </si>
+  <si>
+    <t>Vaslui</t>
+  </si>
+  <si>
+    <t>Iasi</t>
+  </si>
+  <si>
+    <t>Neamt</t>
+  </si>
+  <si>
+    <t>To Bucharest</t>
+  </si>
+  <si>
+    <t>Straight-line distance</t>
+  </si>
+  <si>
+    <t>Cralova</t>
+  </si>
+  <si>
+    <t>Giurgiu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -358,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -368,11 +448,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -724,6 +804,476 @@
       </c>
       <c r="J11">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change 0 - 0.5
</commit_message>
<xml_diff>
--- a/MidAI.xlsx
+++ b/MidAI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Problem1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,13 +485,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -503,16 +503,16 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -549,16 +549,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -590,13 +590,13 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -613,16 +613,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -634,13 +634,13 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -648,13 +648,13 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -663,16 +663,16 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -692,13 +692,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -727,13 +727,13 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -741,19 +741,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -773,16 +773,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -794,13 +794,13 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -812,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change reverse mid AI
</commit_message>
<xml_diff>
--- a/MidAI.xlsx
+++ b/MidAI.xlsx
@@ -435,7 +435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,7 +446,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,322 +485,322 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new ai mid data
</commit_message>
<xml_diff>
--- a/MidAI.xlsx
+++ b/MidAI.xlsx
@@ -435,7 +435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,7 +446,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>